<commit_message>
add example values for arrayexpress-library
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Sequencing_library.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Sequencing_library.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Description</t>
@@ -207,6 +207,33 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>single-end</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000086</t>
+  </si>
+  <si>
+    <t>Genome</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16629</t>
+  </si>
+  <si>
+    <t>Whole Genome Sequencing</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C101294</t>
+  </si>
+  <si>
+    <t>Polymerase Chain Reaction</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
   </si>
 </sst>
 </file>
@@ -889,40 +916,40 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="O2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="R2" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
update building block types
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Sequencing_library.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Sequencing_library.xlsx
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.2</t>
+    <t>1.0.3</t>
   </si>
   <si>
     <t>Description</t>
@@ -176,7 +176,7 @@
     <t>Term Accession Number (DPBO:0000015)</t>
   </si>
   <si>
-    <t>Parameter [library source]</t>
+    <t>Characteristic [library source]</t>
   </si>
   <si>
     <t>Term Source REF (GENEPIO:0001965)</t>
@@ -203,7 +203,7 @@
     <t>Term Accession Number (DPBO:0000036)</t>
   </si>
   <si>
-    <t>Output [Raw Data File]</t>
+    <t>Output [Data]</t>
   </si>
   <si>
     <t/>
@@ -215,7 +215,7 @@
     <t>EFO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/EFO_0004184</t>
+    <t>https://bioregistry.io/EFO:0004184</t>
   </si>
   <si>
     <t>library_construction.txt</t>
@@ -227,25 +227,25 @@
     <t>DPBO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/DPBO_0000086</t>
+    <t>http://purl.org/nfdi4plants/ontology/dpbo/DPBO_0000086</t>
   </si>
   <si>
     <t>Genome</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16629</t>
+    <t>https://bioregistry.io/NCIT:C16629</t>
   </si>
   <si>
     <t>Whole Genome Sequencing</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C101294</t>
+    <t>https://bioregistry.io/NCIT:C101294</t>
   </si>
   <si>
     <t>Polymerase Chain Reaction</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17003</t>
+    <t>https://bioregistry.io/NCIT:C17003</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
     <tableColumn id="6" name="Parameter [library layout]" totalsRowFunction="none"/>
     <tableColumn id="7" name="Term Source REF (DPBO:0000015)" totalsRowFunction="none"/>
     <tableColumn id="8" name="Term Accession Number (DPBO:0000015)" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Parameter [library source]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Characteristic [library source]" totalsRowFunction="none"/>
     <tableColumn id="10" name="Term Source REF (GENEPIO:0001965)" totalsRowFunction="none"/>
     <tableColumn id="11" name="Term Accession Number (GENEPIO:0001965)" totalsRowFunction="none"/>
     <tableColumn id="12" name="Parameter [library strategy]" totalsRowFunction="none"/>
@@ -340,7 +340,7 @@
     <tableColumn id="15" name="Parameter [library selection]" totalsRowFunction="none"/>
     <tableColumn id="16" name="Term Source REF (DPBO:0000036)" totalsRowFunction="none"/>
     <tableColumn id="17" name="Term Accession Number (DPBO:0000036)" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Output [Raw Data File]" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>